<commit_message>
Se termina la parte a de la p2
</commit_message>
<xml_diff>
--- a/T1/lab1-p2-master/ParteA.xlsx
+++ b/T1/lab1-p2-master/ParteA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Desktop\Seguridad\Tareas\Cybersecurity\T1\lab1-p2-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Escritorio\SEGURIDAD\Cybersecurity\T1\lab1-p2-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA95B21C-AA2A-4C38-8B01-6E734D1C6BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06105DC7-EE5B-408B-A31F-185D14A8318F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13311" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4028,8 +4028,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -4152,7 +4160,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -4164,6 +4172,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4196,6 +4205,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Largo de C en</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> función del largo de M</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4209,19 +4248,13 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:effectLst>
-                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="40000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
@@ -8360,16 +8393,76 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-CL"/>
+                  <a:t>Largo</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-CL" baseline="0"/>
+                  <a:t> del mensaje M</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-CL"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:lumMod val="95000"/>
-                <a:alpha val="10000"/>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -8383,8 +8476,9 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -8413,9 +8507,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                  <a:alpha val="10000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -8423,6 +8517,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-CL"/>
+                  <a:t>Largo del mensaje cifrado C</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -8441,8 +8590,9 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -8482,8 +8632,9 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="85000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -8507,28 +8658,17 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:gradFill flip="none" rotWithShape="1">
-      <a:gsLst>
-        <a:gs pos="0">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:gs>
-        <a:gs pos="100000">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="85000"/>
-            <a:lumOff val="15000"/>
-          </a:schemeClr>
-        </a:gs>
-      </a:gsLst>
-      <a:path path="circle">
-        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-      </a:path>
-      <a:tileRect/>
-    </a:gradFill>
-    <a:ln>
-      <a:noFill/>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -8591,33 +8731,35 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="342">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="10000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -8625,44 +8767,37 @@
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:gradFill flip="none" rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="65000"/>
-              <a:lumOff val="35000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="85000"/>
-              <a:lumOff val="15000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:path path="circle">
-          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-        </a:path>
-        <a:tileRect/>
-      </a:gradFill>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -8681,6 +8816,14 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -8769,18 +8912,21 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -8790,20 +8936,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -8817,14 +8963,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -8838,8 +8984,9 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -8851,7 +8998,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
@@ -8864,9 +9011,9 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="10000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -8881,13 +9028,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="5000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -8899,14 +9047,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -8918,13 +9066,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -8933,8 +9082,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -8944,7 +9094,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D>
@@ -8952,7 +9102,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -8960,16 +9110,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -8982,14 +9133,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -9001,19 +9152,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="95000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
-      <a:effectLst>
-        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="40000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
-    </cs:defRPr>
+    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -9022,7 +9166,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
@@ -9037,8 +9181,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -9048,7 +9193,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -9056,9 +9201,9 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -9069,8 +9214,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -9080,7 +9226,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
@@ -9091,15 +9237,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>220980</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>85807</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>109496</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>525780</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>596347</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>55659</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9448,20 +9594,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D666"/>
+  <dimension ref="A1:R666"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.44140625" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -9475,7 +9621,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -9489,7 +9635,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -9503,7 +9649,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -9517,7 +9663,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
@@ -9531,7 +9677,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
@@ -9545,7 +9691,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
@@ -9559,7 +9705,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
@@ -9573,7 +9719,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>18</v>
       </c>
@@ -9587,7 +9733,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -9601,7 +9747,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>22</v>
       </c>
@@ -9615,7 +9761,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>24</v>
       </c>
@@ -9629,7 +9775,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>26</v>
       </c>
@@ -9643,7 +9789,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>28</v>
       </c>
@@ -9657,7 +9803,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>30</v>
       </c>
@@ -9671,7 +9817,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>32</v>
       </c>
@@ -9684,6 +9830,7 @@
       <c r="D16" s="6">
         <v>256</v>
       </c>
+      <c r="R16" s="11"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
@@ -18787,6 +18934,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
se sube el excel con un gráfico más bonito
</commit_message>
<xml_diff>
--- a/T1/lab1-p2-master/ParteA.xlsx
+++ b/T1/lab1-p2-master/ParteA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Escritorio\SEGURIDAD\Cybersecurity\T1\lab1-p2-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06105DC7-EE5B-408B-A31F-185D14A8318F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50538405-0925-4CD8-B8F6-E2A2744075CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13311" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9597,7 +9597,7 @@
   <dimension ref="A1:R666"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>

</xml_diff>